<commit_message>
Bene Addition and Verification
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/BeneficiaryAddition.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/BeneficiaryAddition.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Case</t>
   </si>
@@ -33,24 +33,6 @@
     <t>StatusQuery</t>
   </si>
   <si>
-    <t>BeneficiaryManagement_Bank_Value</t>
-  </si>
-  <si>
-    <t>account_query</t>
-  </si>
-  <si>
-    <t>BeneficiaryManagement_AccountNo_Value</t>
-  </si>
-  <si>
-    <t>BeneficiaryManagement_BeneNick_Value</t>
-  </si>
-  <si>
-    <t>BeneficiaryManagement_PayeeEmail_Value</t>
-  </si>
-  <si>
-    <t>BeneficiaryManagement_PayeeMobileNumber_Value</t>
-  </si>
-  <si>
     <t>03121234567</t>
   </si>
   <si>
@@ -63,10 +45,73 @@
     <t>HBL / Konnect</t>
   </si>
   <si>
-    <t>BEGIN DELETE FROM DC_FUND_TRANSFER_BENEFICIARY TF WHERE TF.ACCOUNT_NO = (SELECT CA.ACCOUNT_NO FROM DC_CUSTOMER_ACCOUNT CA WHERE CA.CUSTOMER_ACCOUNT_ID = '2498940') AND TF.CUSTOMER_INFO_ID = (SELECT CUSTOMER_INFO_ID FROM DC_CUSTOMER_INFO DCI WHERE DCI.CUSTOMER_NAME = 'NAEEMCAR');COMMIT;END;</t>
-  </si>
-  <si>
-    <t>SELECT CA.ACCOUNT_NO FROM DC_CUSTOMER_ACCOUNT CA WHERE CA.CUSTOMER_ACCOUNT_ID = '2498940'</t>
+    <t>account_no</t>
+  </si>
+  <si>
+    <t>Bank_Value</t>
+  </si>
+  <si>
+    <t>BeneNick_Value</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Mobile_No</t>
+  </si>
+  <si>
+    <t>tran_type_query</t>
+  </si>
+  <si>
+    <t>tran_response_query</t>
+  </si>
+  <si>
+    <t>tran_date_query</t>
+  </si>
+  <si>
+    <t>tran_bene_name_query</t>
+  </si>
+  <si>
+    <t>account_no_query</t>
+  </si>
+  <si>
+    <t>email_query</t>
+  </si>
+  <si>
+    <t>mobile_query</t>
+  </si>
+  <si>
+    <t>nick_query</t>
+  </si>
+  <si>
+    <t>07867917196701</t>
+  </si>
+  <si>
+    <t>BEGIN DELETE FROM DC_FUND_TRANSFER_BENEFICIARY TF WHERE TF.ACCOUNT_NO = '{account_number}' AND TF.CUSTOMER_INFO_ID = (SELECT CUSTOMER_INFO_ID FROM DC_CUSTOMER_INFO DCI WHERE DCI.CUSTOMER_NAME = '{customer_name}');COMMIT;END;</t>
+  </si>
+  <si>
+    <t>SELECT AC.DESCRIPTION FROM DC_TRANSACTION_ACTIVITY_CONFIG AC WHERE AC.TRANSACTION_TYPE_ID =(SELECT DT.TRANSACTION_TYPE_ID FROM DC_TRANSACTION DT WHERE DT.TRANSACTION_ID = '</t>
+  </si>
+  <si>
+    <t>SELECT RESPONSE_MESSAGE FROM DC_TRANSACTION DT where DT.TRANSACTION_ID='</t>
+  </si>
+  <si>
+    <t>SELECT CREATED_ON FROM DC_TRANSACTION DT where DT.TRANSACTION_ID='</t>
+  </si>
+  <si>
+    <t>SELECT BENEFICIARY_NAME FROM DC_TRANSACTION DT where DT.TRANSACTION_ID='</t>
+  </si>
+  <si>
+    <t>Select ACCOUNT_NO from DC_FUND_TRANSFER_BENEFICIARY l  where L.CUSTOMER_INFO_ID= ( Select customer_info_id from dc_customer_info K where K.CUSTOMER_NAME = '{customer_name}') and L.ACCOUNT_NO='{account_numer}'</t>
+  </si>
+  <si>
+    <t>Select EMAIL_ADDRESS from DC_FUND_TRANSFER_BENEFICIARY l  where L.CUSTOMER_INFO_ID= ( Select customer_info_id from dc_customer_info K where K.CUSTOMER_NAME = '{customer_name}') and L.ACCOUNT_NO='{account_numer}'</t>
+  </si>
+  <si>
+    <t>Select MOBILE_NO from DC_FUND_TRANSFER_BENEFICIARY l  where L.CUSTOMER_INFO_ID= ( Select customer_info_id from dc_customer_info K where K.CUSTOMER_NAME = '{customer_name}') and L.ACCOUNT_NO='{account_numer}'</t>
+  </si>
+  <si>
+    <t>Select NICK from DC_FUND_TRANSFER_BENEFICIARY l  where L.CUSTOMER_INFO_ID= ( Select customer_info_id from dc_customer_info K where K.CUSTOMER_NAME = '{customer_name}') and L.ACCOUNT_NO='{account_numer}'</t>
   </si>
 </sst>
 </file>
@@ -120,8 +165,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -403,82 +448,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="241.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="185.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="79.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="72.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="215" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="217" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="213" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="206.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>12345</v>
+      <c r="H2" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>